<commit_message>
feat: enhance SpProportionalityValidator with new validation logic and helper functions
</commit_message>
<xml_diff>
--- a/data/input/data_ground_truth_01/proporcionalidades.xlsx
+++ b/data/input/data_ground_truth_01/proporcionalidades.xlsx
@@ -283,7 +283,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,395 +292,395 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="U2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1100015</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="B3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>0.347</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0.211</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.558</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="U3" s="0" t="n">
+      <c r="I3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U3" s="1" t="n">
         <v>0.738</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>0.262</v>
       </c>
-      <c r="W3" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="X3" s="0" t="n">
+      <c r="W3" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="X3" s="1" t="n">
         <v>0.558</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1100023</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>0.347</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.211</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="E4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.558</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Q4" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="R4" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="U4" s="0" t="n">
+      <c r="I4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U4" s="1" t="n">
         <v>0.738</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>0.262</v>
       </c>
-      <c r="W4" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="X4" s="0" t="n">
+      <c r="W4" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="X4" s="1" t="n">
         <v>0.558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1100049</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>0.347</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.211</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.558</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Q5" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="R5" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="S5" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="T5" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="U5" s="0" t="n">
+      <c r="I5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U5" s="1" t="n">
         <v>0.738</v>
       </c>
-      <c r="V5" s="0" t="n">
+      <c r="V5" s="1" t="n">
         <v>0.262</v>
       </c>
-      <c r="W5" s="0" t="n">
+      <c r="W5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="X5" s="0" t="n">
+      <c r="X5" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>1100056</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="C6" s="0" t="n">
+      <c r="B6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>0.347</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>0.211</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>0.442</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="E6" s="1" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>0.558</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="P6" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>0.232</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="U6" s="0" t="n">
+      <c r="I6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="U6" s="1" t="n">
         <v>0.738</v>
       </c>
-      <c r="V6" s="0" t="n">
+      <c r="V6" s="1" t="n">
         <v>0.262</v>
       </c>
-      <c r="W6" s="0" t="s">
+      <c r="W6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X6" s="0" t="s">
+      <c r="X6" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add sum validation for influencing factors in SpProportionalityValidator
</commit_message>
<xml_diff>
--- a/data/input/data_ground_truth_01/proporcionalidades.xlsx
+++ b/data/input/data_ground_truth_01/proporcionalidades.xlsx
@@ -283,7 +283,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -399,7 +399,7 @@
         <v>0.347</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.211</v>
+        <v>887</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0.442</v>
@@ -645,7 +645,7 @@
         <v>0.098</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>0.164</v>
+        <v>35</v>
       </c>
       <c r="M6" s="1" t="n">
         <v>0.506</v>

</xml_diff>